<commit_message>
adding file for descriptions
</commit_message>
<xml_diff>
--- a/Variables Etiquetas.xlsx
+++ b/Variables Etiquetas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15-4JO\Desktop\coding_Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\15-4JO\Desktop\coding_Code\datamining\Proyecto3-Mineria-de-datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F84FB31B-C071-4A76-9D6B-1308283D3706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F2A05A4-198C-4D78-A772-39D32F3F6E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1979" uniqueCount="881">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="881">
   <si>
     <t>Valor</t>
   </si>
@@ -2773,7 +2773,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -2829,6 +2829,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="10">
@@ -3145,8 +3151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C1077"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A312" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView tabSelected="1" topLeftCell="A1024" workbookViewId="0">
+      <selection activeCell="C1036" sqref="C1036"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12547,8 +12553,12 @@
     </row>
     <row r="1040" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1040" s="8"/>
-      <c r="B1040" s="1"/>
-      <c r="C1040" s="2"/>
+      <c r="B1040" s="21">
+        <v>98</v>
+      </c>
+      <c r="C1040" s="20" t="s">
+        <v>856</v>
+      </c>
     </row>
     <row r="1041" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1041" s="8"/>
@@ -12737,6 +12747,13 @@
     </row>
   </sheetData>
   <mergeCells count="19">
+    <mergeCell ref="A410:A421"/>
+    <mergeCell ref="A377:A378"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A3:A24"/>
+    <mergeCell ref="A25:A364"/>
+    <mergeCell ref="A365:A376"/>
+    <mergeCell ref="A379:A409"/>
     <mergeCell ref="A932:A953"/>
     <mergeCell ref="A968:A1008"/>
     <mergeCell ref="A1009:A1039"/>
@@ -12749,13 +12766,6 @@
     <mergeCell ref="A900:A905"/>
     <mergeCell ref="A906:A911"/>
     <mergeCell ref="A912:A931"/>
-    <mergeCell ref="A410:A421"/>
-    <mergeCell ref="A377:A378"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A3:A24"/>
-    <mergeCell ref="A25:A364"/>
-    <mergeCell ref="A365:A376"/>
-    <mergeCell ref="A379:A409"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>